<commit_message>
fix error cancel button
</commit_message>
<xml_diff>
--- a/public/templates/template.xlsx
+++ b/public/templates/template.xlsx
@@ -16,10 +16,10 @@
     <t>name</t>
   </si>
   <si>
-    <t>Latitude</t>
+    <t>latitude</t>
   </si>
   <si>
-    <t>Longitude</t>
+    <t>longitude</t>
   </si>
   <si>
     <t>Cloud Gate - Chicago</t>
@@ -323,6 +323,7 @@
     <col customWidth="1" min="1" max="1" width="21.75"/>
     <col customWidth="1" min="2" max="2" width="20.75"/>
     <col customWidth="1" min="3" max="3" width="24.75"/>
+    <col customWidth="1" min="4" max="4" width="38.25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -384,10 +385,12 @@
     <row r="8">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
+      <c r="D8" s="1"/>
     </row>
     <row r="9">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
+      <c r="D9" s="1"/>
     </row>
     <row r="10">
       <c r="B10" s="4"/>

</xml_diff>